<commit_message>
Subida da primeira versão funcional
</commit_message>
<xml_diff>
--- a/Planilha_COO.xlsx
+++ b/Planilha_COO.xlsx
@@ -14,17 +14,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>COO</t>
+  </si>
+  <si>
+    <t>Serie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -52,13 +63,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -368,7 +385,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -380,31 +397,38 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
+        <v>154</v>
+      </c>
+      <c r="B2" s="5">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
         <v>149</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>150</v>
-      </c>
+      <c r="B3" s="5"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>151</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="B4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>152</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>153</v>
-      </c>
+      <c r="A6" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G9" s="1"/>

</xml_diff>

<commit_message>
Ajuste no caminho para a planilha
</commit_message>
<xml_diff>
--- a/Planilha_COO.xlsx
+++ b/Planilha_COO.xlsx
@@ -35,12 +35,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -72,12 +70,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,7 +381,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -397,35 +393,31 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>154</v>
+      <c r="A2" s="5">
+        <v>25004</v>
       </c>
       <c r="B2" s="5">
-        <v>789</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>149</v>
+      <c r="A3" s="5">
+        <v>25012</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>150</v>
-      </c>
-      <c r="B4" s="5"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
-        <v>100</v>
-      </c>
-      <c r="B5" s="5"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>

</xml_diff>